<commit_message>
cell is a neither term (not context)
</commit_message>
<xml_diff>
--- a/results/chess/chess-stats-identi-20.xlsx
+++ b/results/chess/chess-stats-identi-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desti\Documents\GitHub\P4P\results\chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6579A158-F8DF-4327-8F1A-F8CEEB6CF41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1511C7-0DBA-4D17-A1BF-3DD09A27DFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11505" yWindow="1815" windowWidth="10740" windowHeight="13065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ugrad-009-01-stats-20" sheetId="1" r:id="rId1"/>
@@ -807,7 +807,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.24757281553398058</c:v>
+                  <c:v>0.22815533980582525</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.49606299212598426</c:v>
@@ -872,7 +872,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.28155339805825241</c:v>
+                  <c:v>0.30097087378640774</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.5118110236220472E-2</c:v>
@@ -1975,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,11 +2017,11 @@
       </c>
       <c r="C2">
         <f>raw!B2</f>
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <f>raw!C2</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <f>SUM(B2:D2)</f>
@@ -2033,11 +2033,11 @@
       </c>
       <c r="H2" s="1">
         <f>C2/E2</f>
-        <v>0.24757281553398058</v>
+        <v>0.22815533980582525</v>
       </c>
       <c r="I2" s="1">
         <f>D2/E2</f>
-        <v>0.28155339805825241</v>
+        <v>0.30097087378640774</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2116,11 +2116,11 @@
       </c>
       <c r="C5">
         <f>AVERAGE(C2:C4)</f>
-        <v>61.333333333333336</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <f>AVERAGE(D2:D4)</f>
-        <v>37.333333333333336</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="E5">
         <f>AVERAGE(E2:E4)</f>
@@ -2132,11 +2132,11 @@
       </c>
       <c r="H5" s="1">
         <f>AVERAGE(H2:H4)</f>
-        <v>0.35846312072077818</v>
+        <v>0.35199062881139304</v>
       </c>
       <c r="I5" s="1">
         <f>AVERAGE(I2:I4)</f>
-        <v>0.18647344115344988</v>
+        <v>0.192945933062835</v>
       </c>
     </row>
   </sheetData>
@@ -2150,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2F3F05-6040-485E-941D-4098ABFA4C94}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,10 +2172,10 @@
         <v>97</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>